<commit_message>
Train & Test 1차 완성
</commit_message>
<xml_diff>
--- a/data_kr/KOSPI50 기간설정.xlsx
+++ b/data_kr/KOSPI50 기간설정.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jongh\Graduation_Project\Code_Of_DL\CodeforKorea\data_kr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jongh\Graduation_Project\Code_Of_DL\CodeforKorea\S3CE\data_kr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88FADB57-C622-4525-9FF4-79C16232CBF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{627C3BDA-F723-4D12-B916-CBD50DD6E978}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10850" windowWidth="38620" windowHeight="21100" xr2:uid="{348F6EC0-FDBC-4E5F-A102-0D0A23819889}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{348F6EC0-FDBC-4E5F-A102-0D0A23819889}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="35">
   <si>
     <t>Train_Start</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -155,6 +155,26 @@
   </si>
   <si>
     <t>Q4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2016_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2017_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2019_Q1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3년 2개월</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -264,13 +284,13 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -607,10 +627,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5730C72-01EA-4AC0-A16D-B8A0E1EA9586}">
-  <dimension ref="A1:S8"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -619,22 +639,22 @@
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
       <c r="I1" s="1"/>
@@ -673,22 +693,22 @@
       <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="8" t="s">
         <v>7</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>19</v>
       </c>
       <c r="I2" s="6" t="s">
@@ -727,22 +747,22 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>13</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="6" t="s">
@@ -781,22 +801,22 @@
       <c r="A4" s="2">
         <v>3</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>20</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I4" s="6" t="s">
@@ -835,22 +855,22 @@
       <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="8" t="s">
         <v>14</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I5" s="6" t="s">
@@ -889,22 +909,22 @@
       <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>11</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>8</v>
       </c>
     </row>
@@ -912,18 +932,18 @@
       <c r="A7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="9"/>
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="7"/>
+      <c r="G7" s="9"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.4">
       <c r="A8" s="4"/>
@@ -934,11 +954,194 @@
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
     </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>15</v>
+      </c>
+      <c r="K11">
+        <v>19</v>
+      </c>
+      <c r="L11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A12" s="2">
+        <v>2</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12">
+        <v>5</v>
+      </c>
+      <c r="J12">
+        <v>19</v>
+      </c>
+      <c r="K12">
+        <v>23</v>
+      </c>
+      <c r="L12">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A13" s="2">
+        <v>3</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13">
+        <v>9</v>
+      </c>
+      <c r="J13">
+        <v>23</v>
+      </c>
+      <c r="K13">
+        <v>27</v>
+      </c>
+      <c r="L13">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A14" s="2">
+        <v>4</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <v>13</v>
+      </c>
+      <c r="J14">
+        <v>27</v>
+      </c>
+      <c r="K14">
+        <v>31</v>
+      </c>
+      <c r="L14">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.4">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G15" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="6">
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="D7:E7"/>
     <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F15:G15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>